<commit_message>
Tests and small fixes
</commit_message>
<xml_diff>
--- a/Files/dictDirectAccess_template.xlsx
+++ b/Files/dictDirectAccess_template.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Ценовой лист</t>
   </si>
@@ -35,6 +35,12 @@
   </si>
   <si>
     <t>Value::IntStringDict[42]</t>
+  </si>
+  <si>
+    <t>Value::InnerPriceList.PriceListsDict["price"].Type</t>
+  </si>
+  <si>
+    <t>Value::InnerPriceList.IntStringDict[25]</t>
   </si>
 </sst>
 </file>
@@ -757,7 +763,7 @@
   <dimension ref="A1:S20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13:C13"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -908,7 +914,9 @@
       <c r="B9" s="56"/>
       <c r="C9" s="15"/>
       <c r="D9" s="16"/>
-      <c r="E9" s="16"/>
+      <c r="E9" s="10" t="s">
+        <v>8</v>
+      </c>
       <c r="F9" s="57"/>
       <c r="G9" s="57"/>
       <c r="H9"/>
@@ -921,7 +929,9 @@
       <c r="B10" s="56"/>
       <c r="C10" s="15"/>
       <c r="D10" s="16"/>
-      <c r="E10" s="16"/>
+      <c r="E10" s="10" t="s">
+        <v>7</v>
+      </c>
       <c r="F10" s="57"/>
       <c r="G10" s="57"/>
       <c r="H10"/>

</xml_diff>